<commit_message>
get report API backend
</commit_message>
<xml_diff>
--- a/backend/report/Estimation.xlsx
+++ b/backend/report/Estimation.xlsx
@@ -648,7 +648,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -664,8 +664,14 @@
       <c r="E5">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -681,8 +687,14 @@
       <c r="E6">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -698,8 +710,14 @@
       <c r="E7">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>4000</v>
+      </c>
+      <c r="G7">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -714,6 +732,12 @@
       </c>
       <c r="E8">
         <v>3.9</v>
+      </c>
+      <c r="F8">
+        <v>5000</v>
+      </c>
+      <c r="G8">
+        <v>6500</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Summary data updated in Excel download
</commit_message>
<xml_diff>
--- a/backend/report/Estimation.xlsx
+++ b/backend/report/Estimation.xlsx
@@ -5,13 +5,15 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Estimation Detail" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Estimation Summary" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Resource Planning" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="70">
   <si>
     <t>Requirement</t>
   </si>
@@ -149,19 +151,94 @@
   </si>
   <si>
     <t>sdfds</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total Contingency</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Calculative</t>
+  </si>
+  <si>
+    <t>Contingency</t>
+  </si>
+  <si>
+    <t>sads 10 % of  MANUAL TESTING, UAT</t>
+  </si>
+  <si>
+    <t>sadsa 12 % of  PROD, AUTOMATION</t>
+  </si>
+  <si>
+    <t>sdsad(Manual)</t>
+  </si>
+  <si>
+    <t>etest 10 % of  DESIGN, MANUAL TESTING</t>
+  </si>
+  <si>
+    <t>Estimation Total</t>
+  </si>
+  <si>
+    <t>S No.</t>
+  </si>
+  <si>
+    <t>Allocation%</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Skills(Effort &amp; Summary Attributes)</t>
+  </si>
+  <si>
+    <t>Cost/Hr($)</t>
+  </si>
+  <si>
+    <t>Price/Hr($)</t>
+  </si>
+  <si>
+    <t>Cost($)</t>
+  </si>
+  <si>
+    <t>Price($)</t>
+  </si>
+  <si>
+    <t>Sr Lead</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>sdsad</t>
+  </si>
+  <si>
+    <t>sads</t>
+  </si>
+  <si>
+    <t>sadsa</t>
+  </si>
+  <si>
+    <t>etest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,8 +261,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -201,6 +279,62 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="MyTable" displayName="MyTable" ref="A1:O7" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:O7">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+    <filterColumn colId="14" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="15">
+    <tableColumn id="1" name="Tag" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="About Us" totalsRowFunction="none"/>
+    <tableColumn id="3" name="About Us Contingency" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Frontend" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Frontend Contingency" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Homepage" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Homepage Contingency" totalsRowFunction="none"/>
+    <tableColumn id="8" name="Project Manager" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Project Manager Contingency" totalsRowFunction="none"/>
+    <tableColumn id="10" name="QnA" totalsRowFunction="none"/>
+    <tableColumn id="11" name="QnA Contingency" totalsRowFunction="none"/>
+    <tableColumn id="12" name="UI" totalsRowFunction="none"/>
+    <tableColumn id="13" name="UI Contingency" totalsRowFunction="none"/>
+    <tableColumn id="14" name="Total" totalsRowFunction="none"/>
+    <tableColumn id="15" name="Total Contingency" totalsRowFunction="none"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" name="MyTable2" displayName="MyTable2" ref="A20:C25" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A20:C25">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Calculative" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Contingency" totalsRowFunction="none"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -533,49 +667,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -874,6 +1008,1153 @@
       </c>
       <c r="E16">
         <v>7.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>14.3</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>37.7</v>
+      </c>
+      <c r="D3">
+        <v>9011</v>
+      </c>
+      <c r="E3">
+        <v>11714.3</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>36.4</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>7.8</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>6.5</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>9.1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>14.3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>84</v>
+      </c>
+      <c r="C7">
+        <v>109.2</v>
+      </c>
+      <c r="D7">
+        <v>9024</v>
+      </c>
+      <c r="E7">
+        <v>11731.2</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>4.5</v>
+      </c>
+      <c r="C21">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22">
+        <v>2.76</v>
+      </c>
+      <c r="C22">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24">
+        <v>907.4</v>
+      </c>
+      <c r="C24">
+        <v>1179.62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25">
+        <v>10032.66</v>
+      </c>
+      <c r="C25">
+        <v>13042.46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H33"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="4" width="30" customWidth="1"/>
+    <col min="5" max="8" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>800</v>
+      </c>
+      <c r="H2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
+      <c r="H3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="H4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>200</v>
+      </c>
+      <c r="H5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>200</v>
+      </c>
+      <c r="H6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>200</v>
+      </c>
+      <c r="H7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>800</v>
+      </c>
+      <c r="H9">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>800</v>
+      </c>
+      <c r="H10">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>30</v>
+      </c>
+      <c r="G11">
+        <v>800</v>
+      </c>
+      <c r="H11">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>30</v>
+      </c>
+      <c r="G12">
+        <v>800</v>
+      </c>
+      <c r="H12">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <v>800</v>
+      </c>
+      <c r="H13">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>800</v>
+      </c>
+      <c r="H14">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>30</v>
+      </c>
+      <c r="G15">
+        <v>800</v>
+      </c>
+      <c r="H15">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>30</v>
+      </c>
+      <c r="G16">
+        <v>800</v>
+      </c>
+      <c r="H16">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>30</v>
+      </c>
+      <c r="G17">
+        <v>800</v>
+      </c>
+      <c r="H17">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>30</v>
+      </c>
+      <c r="G18">
+        <v>800</v>
+      </c>
+      <c r="H18">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>20</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <v>800</v>
+      </c>
+      <c r="H19">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>30</v>
+      </c>
+      <c r="G20">
+        <v>800</v>
+      </c>
+      <c r="H20">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>30</v>
+      </c>
+      <c r="G21">
+        <v>200</v>
+      </c>
+      <c r="H21">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>30</v>
+      </c>
+      <c r="G22">
+        <v>200</v>
+      </c>
+      <c r="H22">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <v>30</v>
+      </c>
+      <c r="G23">
+        <v>200</v>
+      </c>
+      <c r="H23">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24">
+        <v>20</v>
+      </c>
+      <c r="F24">
+        <v>30</v>
+      </c>
+      <c r="G24">
+        <v>600</v>
+      </c>
+      <c r="H24">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25">
+        <v>30</v>
+      </c>
+      <c r="G25">
+        <v>600</v>
+      </c>
+      <c r="H25">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
+      </c>
+      <c r="G26">
+        <v>600</v>
+      </c>
+      <c r="H26">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+      <c r="G27">
+        <v>800</v>
+      </c>
+      <c r="H27">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="G28">
+        <v>200</v>
+      </c>
+      <c r="H28">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29">
+        <v>20</v>
+      </c>
+      <c r="F29">
+        <v>30</v>
+      </c>
+      <c r="G29">
+        <v>600</v>
+      </c>
+      <c r="H29">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>20</v>
+      </c>
+      <c r="F30">
+        <v>30</v>
+      </c>
+      <c r="G30">
+        <v>600</v>
+      </c>
+      <c r="H30">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>75</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>20</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <v>600</v>
+      </c>
+      <c r="H31">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>100</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32">
+        <v>800</v>
+      </c>
+      <c r="H32">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33">
+        <v>20</v>
+      </c>
+      <c r="F33">
+        <v>30</v>
+      </c>
+      <c r="G33">
+        <v>600</v>
+      </c>
+      <c r="H33">
+        <v>900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>